<commit_message>
Add get similiar when not found FAQ
</commit_message>
<xml_diff>
--- a/templates/chatbot/data/en/system_chatbot_UI_text.xlsx
+++ b/templates/chatbot/data/en/system_chatbot_UI_text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\24.exceedone\Manual5-1\srcexment\templates\chatbot\data\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91BE2DB-A658-4A9D-B0A0-E041A74762C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7049242-A461-48A0-828E-009A4832DFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="system_chatbot_UI_text" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -134,6 +134,15 @@
   </si>
   <si>
     <t>Farewell message shown when the user ends the conversation.</t>
+  </si>
+  <si>
+    <t>error_message</t>
+  </si>
+  <si>
+    <t>Error message shown when there is no relevant data for the user's question. Encourages the user to ask a more specific question.</t>
+  </si>
+  <si>
+    <t>Sorry, there is no data available related to your question. If you could ask a more specific question, I believe I can assist you better.</t>
   </si>
 </sst>
 </file>
@@ -473,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -669,6 +678,20 @@
         <v>37</v>
       </c>
     </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>